<commit_message>
data appended for new hotels
</commit_message>
<xml_diff>
--- a/scrapers/TA/scrapes/1. Run/Excel_per_Hotel /Dubai_Prices_appended.xlsx
+++ b/scrapers/TA/scrapes/1. Run/Excel_per_Hotel /Dubai_Prices_appended.xlsx
@@ -1,20 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
+  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TobiasRordorf/Desktop/UNI/MBI HSG/4. Semester/Python/GitHub/hotelierchallenge/scrapers/TA/scrapes/1. Run/Excel_per_Hotel /"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F000A81-E827-5F4E-AD9D-3A7915D1877D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="20820" windowHeight="14960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="331">
   <si>
     <t>price_per_night</t>
   </si>
@@ -22,49 +36,49 @@
     <t>Datum</t>
   </si>
   <si>
-    <t xml:space="preserve"> 527</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 587</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 295</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 526</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 528</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 296</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 586</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 294</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 464</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 529</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 465</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 585</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 516</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 515</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 653</t>
+    <t> 527</t>
+  </si>
+  <si>
+    <t> 587</t>
+  </si>
+  <si>
+    <t> 295</t>
+  </si>
+  <si>
+    <t> 526</t>
+  </si>
+  <si>
+    <t> 528</t>
+  </si>
+  <si>
+    <t> 296</t>
+  </si>
+  <si>
+    <t> 586</t>
+  </si>
+  <si>
+    <t> 294</t>
+  </si>
+  <si>
+    <t> 464</t>
+  </si>
+  <si>
+    <t> 529</t>
+  </si>
+  <si>
+    <t> 465</t>
+  </si>
+  <si>
+    <t> 585</t>
+  </si>
+  <si>
+    <t> 516</t>
+  </si>
+  <si>
+    <t> 515</t>
+  </si>
+  <si>
+    <t> 653</t>
   </si>
   <si>
     <t>2019-04-05 14-01</t>
@@ -1012,8 +1026,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1065,22 +1079,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1122,7 +1145,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1154,9 +1177,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1188,6 +1229,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1363,14 +1422,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C315"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Tabelle1"/>
+  <dimension ref="A1:E315"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1378,128 +1443,167 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
+      <c r="B2">
+        <v>527</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
+      <c r="B3">
+        <v>587</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="E3">
+        <f>(B3-B2)/B2</f>
+        <v>0.11385199240986717</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
+      <c r="B4">
+        <v>527</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="E4">
+        <f>(B4-B3)/B3</f>
+        <v>-0.10221465076660988</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
+      <c r="B5">
+        <v>295</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="E5">
+        <f t="shared" ref="E5:E11" si="0">(B5-B4)/B4</f>
+        <v>-0.44022770398481975</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
+      <c r="B6">
+        <v>526</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.7830508474576271</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
+      <c r="B7">
+        <v>528</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>3.8022813688212928E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>4</v>
+      <c r="B8">
+        <v>295</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>-0.44128787878787878</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>5</v>
+      <c r="B9">
+        <v>526</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.7830508474576271</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>2</v>
+      <c r="B10">
+        <v>527</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>1.9011406844106464E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>7</v>
+      <c r="B11">
+        <v>596</v>
       </c>
       <c r="C11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.13092979127134724</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1510,7 +1614,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1521,7 +1625,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1532,7 +1636,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1543,7 +1647,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1554,7 +1658,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1565,7 +1669,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1576,7 +1680,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1587,7 +1691,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1598,7 +1702,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1609,7 +1713,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1620,7 +1724,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1631,7 +1735,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1642,7 +1746,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1653,7 +1757,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1664,7 +1768,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1675,7 +1779,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1686,7 +1790,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1697,7 +1801,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1708,7 +1812,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1719,7 +1823,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1730,7 +1834,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1741,7 +1845,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1752,7 +1856,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1763,7 +1867,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1774,7 +1878,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1785,7 +1889,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1796,7 +1900,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1807,7 +1911,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1818,7 +1922,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1829,7 +1933,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1840,7 +1944,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1851,7 +1955,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1862,7 +1966,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1873,7 +1977,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1884,7 +1988,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1895,7 +1999,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1906,7 +2010,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1917,7 +2021,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1928,7 +2032,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1939,7 +2043,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1950,7 +2054,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1961,7 +2065,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1972,7 +2076,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1983,7 +2087,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1994,7 +2098,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2005,7 +2109,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2016,7 +2120,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2027,7 +2131,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2038,7 +2142,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2049,7 +2153,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2060,7 +2164,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2071,7 +2175,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2082,7 +2186,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2093,7 +2197,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2104,7 +2208,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2115,7 +2219,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2126,7 +2230,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2137,7 +2241,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2148,7 +2252,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2159,7 +2263,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2170,7 +2274,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2181,7 +2285,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2192,7 +2296,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2203,7 +2307,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2214,7 +2318,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2225,7 +2329,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -2236,7 +2340,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2247,7 +2351,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2258,7 +2362,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2269,7 +2373,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2280,7 +2384,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2291,7 +2395,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2302,7 +2406,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -2313,7 +2417,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -2324,7 +2428,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -2335,7 +2439,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -2346,7 +2450,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -2357,7 +2461,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -2368,7 +2472,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -2379,7 +2483,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -2390,7 +2494,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -2401,7 +2505,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -2412,7 +2516,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -2423,7 +2527,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -2434,7 +2538,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -2445,7 +2549,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -2456,7 +2560,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -2467,7 +2571,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -2478,7 +2582,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -2489,7 +2593,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -2500,7 +2604,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -2511,7 +2615,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -2522,7 +2626,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -2533,7 +2637,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -2544,7 +2648,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -2555,7 +2659,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -2566,7 +2670,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -2577,7 +2681,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -2588,7 +2692,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -2599,7 +2703,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -2610,7 +2714,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -2621,7 +2725,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -2632,7 +2736,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -2643,7 +2747,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -2654,7 +2758,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -2665,7 +2769,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -2676,7 +2780,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -2687,7 +2791,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -2698,7 +2802,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -2709,7 +2813,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -2720,7 +2824,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="124" spans="1:3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -2731,7 +2835,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -2742,7 +2846,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -2753,7 +2857,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -2764,7 +2868,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="128" spans="1:3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -2775,7 +2879,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -2786,7 +2890,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -2797,7 +2901,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -2808,7 +2912,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -2819,7 +2923,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -2830,7 +2934,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -2841,7 +2945,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -2852,7 +2956,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="136" spans="1:3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -2863,7 +2967,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -2874,7 +2978,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -2885,7 +2989,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="139" spans="1:3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -2896,7 +3000,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -2907,7 +3011,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="141" spans="1:3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -2918,7 +3022,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="142" spans="1:3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -2929,7 +3033,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="143" spans="1:3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -2940,7 +3044,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -2951,7 +3055,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -2962,7 +3066,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -2973,7 +3077,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -2984,7 +3088,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -2995,7 +3099,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="149" spans="1:3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -3006,7 +3110,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="150" spans="1:3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -3017,7 +3121,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="151" spans="1:3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -3028,7 +3132,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="152" spans="1:3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -3039,7 +3143,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="153" spans="1:3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -3050,7 +3154,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -3061,7 +3165,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="155" spans="1:3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -3072,7 +3176,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="156" spans="1:3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -3083,7 +3187,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="157" spans="1:3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -3094,7 +3198,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="158" spans="1:3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -3105,7 +3209,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="159" spans="1:3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -3116,7 +3220,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="160" spans="1:3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -3127,7 +3231,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="161" spans="1:3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -3138,7 +3242,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="162" spans="1:3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -3149,7 +3253,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="163" spans="1:3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -3160,7 +3264,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="164" spans="1:3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -3171,7 +3275,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="165" spans="1:3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -3182,7 +3286,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="166" spans="1:3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -3193,7 +3297,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="167" spans="1:3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -3204,7 +3308,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="168" spans="1:3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -3215,7 +3319,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="169" spans="1:3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -3226,7 +3330,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="170" spans="1:3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -3237,7 +3341,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="171" spans="1:3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -3248,7 +3352,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="172" spans="1:3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -3259,7 +3363,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="173" spans="1:3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -3270,7 +3374,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="174" spans="1:3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -3281,7 +3385,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="175" spans="1:3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -3292,7 +3396,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="176" spans="1:3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -3303,7 +3407,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="177" spans="1:3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -3314,7 +3418,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="178" spans="1:3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -3325,7 +3429,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="179" spans="1:3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -3336,7 +3440,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="180" spans="1:3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -3347,7 +3451,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="181" spans="1:3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -3358,7 +3462,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="182" spans="1:3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -3369,7 +3473,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="183" spans="1:3">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -3380,7 +3484,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="184" spans="1:3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -3391,7 +3495,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="185" spans="1:3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -3402,7 +3506,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="186" spans="1:3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -3413,7 +3517,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="187" spans="1:3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -3424,7 +3528,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="188" spans="1:3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -3435,7 +3539,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="189" spans="1:3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -3446,7 +3550,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="190" spans="1:3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -3457,7 +3561,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="191" spans="1:3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -3468,7 +3572,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="192" spans="1:3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -3479,7 +3583,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="193" spans="1:3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -3490,7 +3594,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="194" spans="1:3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -3501,7 +3605,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="195" spans="1:3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -3512,7 +3616,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="196" spans="1:3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -3523,7 +3627,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="197" spans="1:3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -3534,7 +3638,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="198" spans="1:3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -3545,7 +3649,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="199" spans="1:3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -3556,7 +3660,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="200" spans="1:3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -3567,7 +3671,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="201" spans="1:3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -3578,7 +3682,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="202" spans="1:3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -3589,7 +3693,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="203" spans="1:3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -3600,7 +3704,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="204" spans="1:3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -3611,7 +3715,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="205" spans="1:3">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -3622,7 +3726,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="206" spans="1:3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -3633,7 +3737,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="207" spans="1:3">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -3644,7 +3748,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="208" spans="1:3">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -3655,7 +3759,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="209" spans="1:3">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -3666,7 +3770,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="210" spans="1:3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -3677,7 +3781,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="211" spans="1:3">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -3688,7 +3792,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="212" spans="1:3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -3699,7 +3803,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="213" spans="1:3">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -3710,7 +3814,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="214" spans="1:3">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -3721,7 +3825,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="215" spans="1:3">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -3732,7 +3836,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="216" spans="1:3">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -3743,7 +3847,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="217" spans="1:3">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -3754,7 +3858,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="218" spans="1:3">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -3765,7 +3869,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="219" spans="1:3">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -3776,7 +3880,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="220" spans="1:3">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -3787,7 +3891,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="221" spans="1:3">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -3798,7 +3902,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="222" spans="1:3">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -3809,7 +3913,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="223" spans="1:3">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -3820,7 +3924,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="224" spans="1:3">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -3831,7 +3935,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="225" spans="1:3">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -3842,7 +3946,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="226" spans="1:3">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -3853,7 +3957,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="227" spans="1:3">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -3864,7 +3968,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="228" spans="1:3">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -3875,7 +3979,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="229" spans="1:3">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -3886,7 +3990,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="230" spans="1:3">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -3897,7 +4001,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="231" spans="1:3">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -3908,7 +4012,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="232" spans="1:3">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -3919,7 +4023,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="233" spans="1:3">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -3930,7 +4034,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="234" spans="1:3">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -3941,7 +4045,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="235" spans="1:3">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -3952,7 +4056,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="236" spans="1:3">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -3963,7 +4067,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="237" spans="1:3">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -3974,7 +4078,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="238" spans="1:3">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -3985,7 +4089,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="239" spans="1:3">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -3996,7 +4100,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="240" spans="1:3">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -4007,7 +4111,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="241" spans="1:3">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -4018,7 +4122,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="242" spans="1:3">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -4029,7 +4133,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="243" spans="1:3">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -4040,7 +4144,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="244" spans="1:3">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -4051,7 +4155,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="245" spans="1:3">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -4062,7 +4166,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="246" spans="1:3">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -4073,7 +4177,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="247" spans="1:3">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -4084,7 +4188,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="248" spans="1:3">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -4095,7 +4199,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="249" spans="1:3">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>247</v>
       </c>
@@ -4106,7 +4210,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="250" spans="1:3">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -4117,7 +4221,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="251" spans="1:3">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>249</v>
       </c>
@@ -4128,7 +4232,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="252" spans="1:3">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -4139,7 +4243,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="253" spans="1:3">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -4150,7 +4254,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="254" spans="1:3">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>252</v>
       </c>
@@ -4161,7 +4265,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="255" spans="1:3">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>253</v>
       </c>
@@ -4172,7 +4276,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="256" spans="1:3">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>254</v>
       </c>
@@ -4183,7 +4287,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="257" spans="1:3">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>255</v>
       </c>
@@ -4194,7 +4298,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="258" spans="1:3">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>256</v>
       </c>
@@ -4205,7 +4309,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="259" spans="1:3">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>257</v>
       </c>
@@ -4216,7 +4320,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="260" spans="1:3">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>258</v>
       </c>
@@ -4227,7 +4331,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="261" spans="1:3">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>259</v>
       </c>
@@ -4238,7 +4342,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="262" spans="1:3">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>260</v>
       </c>
@@ -4249,7 +4353,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="263" spans="1:3">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>261</v>
       </c>
@@ -4260,7 +4364,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="264" spans="1:3">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>262</v>
       </c>
@@ -4271,7 +4375,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="265" spans="1:3">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>263</v>
       </c>
@@ -4282,7 +4386,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="266" spans="1:3">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>264</v>
       </c>
@@ -4293,7 +4397,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="267" spans="1:3">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>265</v>
       </c>
@@ -4304,7 +4408,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="268" spans="1:3">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>266</v>
       </c>
@@ -4315,7 +4419,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="269" spans="1:3">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
         <v>267</v>
       </c>
@@ -4326,7 +4430,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="270" spans="1:3">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
         <v>268</v>
       </c>
@@ -4337,7 +4441,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="271" spans="1:3">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
         <v>269</v>
       </c>
@@ -4348,7 +4452,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="272" spans="1:3">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272" s="1">
         <v>270</v>
       </c>
@@ -4359,7 +4463,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="273" spans="1:3">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A273" s="1">
         <v>271</v>
       </c>
@@ -4370,7 +4474,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="274" spans="1:3">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A274" s="1">
         <v>272</v>
       </c>
@@ -4381,7 +4485,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="275" spans="1:3">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A275" s="1">
         <v>273</v>
       </c>
@@ -4392,7 +4496,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="276" spans="1:3">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A276" s="1">
         <v>274</v>
       </c>
@@ -4403,7 +4507,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="277" spans="1:3">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A277" s="1">
         <v>275</v>
       </c>
@@ -4414,7 +4518,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="278" spans="1:3">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A278" s="1">
         <v>276</v>
       </c>
@@ -4425,7 +4529,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="279" spans="1:3">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A279" s="1">
         <v>277</v>
       </c>
@@ -4436,7 +4540,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="280" spans="1:3">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
         <v>278</v>
       </c>
@@ -4447,7 +4551,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="281" spans="1:3">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A281" s="1">
         <v>279</v>
       </c>
@@ -4458,7 +4562,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="282" spans="1:3">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A282" s="1">
         <v>280</v>
       </c>
@@ -4469,7 +4573,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="283" spans="1:3">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A283" s="1">
         <v>281</v>
       </c>
@@ -4480,7 +4584,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="284" spans="1:3">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A284" s="1">
         <v>282</v>
       </c>
@@ -4491,7 +4595,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="285" spans="1:3">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A285" s="1">
         <v>283</v>
       </c>
@@ -4502,7 +4606,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="286" spans="1:3">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286" s="1">
         <v>284</v>
       </c>
@@ -4513,7 +4617,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="287" spans="1:3">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A287" s="1">
         <v>285</v>
       </c>
@@ -4524,7 +4628,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="288" spans="1:3">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A288" s="1">
         <v>286</v>
       </c>
@@ -4535,7 +4639,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="289" spans="1:3">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A289" s="1">
         <v>287</v>
       </c>
@@ -4546,7 +4650,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="290" spans="1:3">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A290" s="1">
         <v>288</v>
       </c>
@@ -4557,7 +4661,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="291" spans="1:3">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A291" s="1">
         <v>289</v>
       </c>
@@ -4568,7 +4672,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="292" spans="1:3">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A292" s="1">
         <v>290</v>
       </c>
@@ -4579,7 +4683,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="293" spans="1:3">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A293" s="1">
         <v>291</v>
       </c>
@@ -4590,7 +4694,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="294" spans="1:3">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A294" s="1">
         <v>292</v>
       </c>
@@ -4601,7 +4705,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="295" spans="1:3">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A295" s="1">
         <v>293</v>
       </c>
@@ -4612,7 +4716,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="296" spans="1:3">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A296" s="1">
         <v>294</v>
       </c>
@@ -4623,7 +4727,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="297" spans="1:3">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A297" s="1">
         <v>295</v>
       </c>
@@ -4634,7 +4738,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="298" spans="1:3">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A298" s="1">
         <v>296</v>
       </c>
@@ -4645,7 +4749,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="299" spans="1:3">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A299" s="1">
         <v>297</v>
       </c>
@@ -4656,7 +4760,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="300" spans="1:3">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A300" s="1">
         <v>298</v>
       </c>
@@ -4667,7 +4771,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="301" spans="1:3">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A301" s="1">
         <v>299</v>
       </c>
@@ -4678,7 +4782,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="302" spans="1:3">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A302" s="1">
         <v>300</v>
       </c>
@@ -4689,7 +4793,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="303" spans="1:3">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A303" s="1">
         <v>301</v>
       </c>
@@ -4700,7 +4804,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="304" spans="1:3">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A304" s="1">
         <v>302</v>
       </c>
@@ -4711,7 +4815,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="305" spans="1:3">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A305" s="1">
         <v>303</v>
       </c>
@@ -4722,7 +4826,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="306" spans="1:3">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A306" s="1">
         <v>304</v>
       </c>
@@ -4733,7 +4837,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="307" spans="1:3">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A307" s="1">
         <v>305</v>
       </c>
@@ -4744,7 +4848,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="308" spans="1:3">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A308" s="1">
         <v>306</v>
       </c>
@@ -4755,7 +4859,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="309" spans="1:3">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A309" s="1">
         <v>307</v>
       </c>
@@ -4766,7 +4870,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="310" spans="1:3">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A310" s="1">
         <v>308</v>
       </c>
@@ -4777,7 +4881,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="311" spans="1:3">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A311" s="1">
         <v>309</v>
       </c>
@@ -4788,7 +4892,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="312" spans="1:3">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A312" s="1">
         <v>310</v>
       </c>
@@ -4799,7 +4903,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="313" spans="1:3">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A313" s="1">
         <v>311</v>
       </c>
@@ -4810,7 +4914,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="314" spans="1:3">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A314" s="1">
         <v>312</v>
       </c>
@@ -4821,7 +4925,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="315" spans="1:3">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A315" s="1">
         <v>313</v>
       </c>

</xml_diff>